<commit_message>
OSIS-3981 Fixed tests suite à modification du modèle Person (field email not null)
 Modifications qui seront validées :
	modifié :         assessments/tests/resources/correct_score_sheet_one_empty_email.xlsx
	modifié :         assessments/tests/views/test_upload_xls_utils.py
</commit_message>
<xml_diff>
--- a/assessments/tests/resources/correct_score_sheet_one_empty_email.xlsx
+++ b/assessments/tests/resources/correct_score_sheet_one_empty_email.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t xml:space="preserve">2017-18 – LOSIS1211</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
@@ -219,12 +222,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -296,8 +299,8 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -415,12 +418,14 @@
       <c r="G12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="I12" s="0" t="n">
         <v>16</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L12" s="2" t="n">
         <v>21</v>
@@ -440,22 +445,22 @@
         <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="L13" s="2" t="n">
         <v>18</v>

</xml_diff>